<commit_message>
Changing README.md and RevenueINputs to eliminate empty revenue tabs
</commit_message>
<xml_diff>
--- a/Data/Input/RevenueInputs.xlsx
+++ b/Data/Input/RevenueInputs.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcbreslin\Dropbox (Personal)\ProjectionsFreemium\ProjectionsFreemium\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3BC28A-7D84-460E-A22E-15B68917D081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF652107-1A4A-467D-9296-9430F6FB2BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{437B8FF6-8FA9-4AF9-AD24-2CDE80E4D88A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{437B8FF6-8FA9-4AF9-AD24-2CDE80E4D88A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Existing - Empty" sheetId="2" r:id="rId1"/>
-    <sheet name="Contracts - Empty" sheetId="9" r:id="rId2"/>
-    <sheet name="New - Empty" sheetId="8" r:id="rId3"/>
-    <sheet name="Existing" sheetId="10" r:id="rId4"/>
-    <sheet name="Contracts" sheetId="11" r:id="rId5"/>
-    <sheet name="New" sheetId="12" r:id="rId6"/>
+    <sheet name="Existing" sheetId="10" r:id="rId1"/>
+    <sheet name="Contracts" sheetId="11" r:id="rId2"/>
+    <sheet name="New" sheetId="12" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Contracts!$A$1:$I$114</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Contracts - Empty'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Existing!$A$1:$K$1910</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Existing - Empty'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Contracts!$A$1:$I$114</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Existing!$A$1:$K$1910</definedName>
     <definedName name="AS2DocOpenMode" hidden="1">"AS2DocumentEdit"</definedName>
     <definedName name="CIQWBGuid" hidden="1">"7bb3c612-6d5b-4e4a-a29a-b7b19c30c524"</definedName>
     <definedName name="client_lookup">#REF!</definedName>
@@ -51,8 +46,7 @@
     <definedName name="IQ_TODAY" hidden="1">0</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
     <definedName name="Product_lookup">#REF!</definedName>
-    <definedName name="Z_7C183D42_5B74_4236_9140_BCE42AAF0975_.wvu.FilterData" localSheetId="3" hidden="1">Existing!$B$1:$J$1923</definedName>
-    <definedName name="Z_7C183D42_5B74_4236_9140_BCE42AAF0975_.wvu.FilterData" localSheetId="0" hidden="1">'Existing - Empty'!$B$1:$J$1</definedName>
+    <definedName name="Z_7C183D42_5B74_4236_9140_BCE42AAF0975_.wvu.FilterData" localSheetId="0" hidden="1">Existing!$B$1:$J$1923</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -75,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6410" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6381" uniqueCount="326">
   <si>
     <t>Recurring</t>
   </si>
@@ -1779,189 +1773,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4743E87-021F-4B4C-BABC-3FE8096B71F6}">
-  <sheetPr codeName="Sheet23">
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="11" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="4" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="12.42578125" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>324</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{D4743E87-021F-4B4C-BABC-3FE8096B71F6}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413C4774-BBFA-4E53-9F2D-694570D927FF}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="14.42578125" style="1"/>
-    <col min="12" max="12" width="14.42578125" style="20"/>
-    <col min="13" max="16384" width="14.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>324</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{413C4774-BBFA-4E53-9F2D-694570D927FF}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BA079C-F0B1-4635-A5DD-B90B9DA6B91A}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>324</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12073B43-85A6-4466-9D7D-8B7DA231873D}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Q1925"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -76660,7 +76478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C657EAD3-B39F-4AA2-9A93-F5A444D61A65}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -80086,11 +79904,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B36A6E58-10D3-4273-BB5D-2ECA4E2753FA}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>